<commit_message>
Add job scraping functionality using BeautifulSoup
- Implemented a function to scrape job listings from HTML content.
- Extracted job title, company name, location, salary, requirements, and job link.
- Added example usage to read HTML from a file and print the scraped job details.
</commit_message>
<xml_diff>
--- a/OCC_especialista-en-implementacion-de-software.xlsx
+++ b/OCC_especialista-en-implementacion-de-software.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -444,6 +444,36 @@
           <t>Enlace</t>
         </is>
       </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Título</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Ubicación</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Paga</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Empresa</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>I_Detalles</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>I_Descripción</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -453,19 +483,96 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>https://www.occ.com.mx/empleos/de-especialista-en-implementacion-de-software/?jobid=20652795</t>
-        </is>
-      </c>
+          <t>https://www.occ.com.mx/empleos/de-especialista-en-implementacion-de-software/?jobid=20642450</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Postularme</t>
+          <t>Postularme
+Esta es una vacante externa, deberás completar el proceso en el sitio de la empresa.
+Postularme
+Postularme
+Postularme</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>https://www.occ.com.mx/empleos/de-especialista-en-implementacion-de-software/?jobid=20612197</t>
+          <t>https://www.occ.com.mx/empleos/de-especialista-en-implementacion-de-software/?jobid=20652795</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Especialista Técnico en Integración/Implementación de Sistemas</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Ciudad de México</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Si el reclutador te contacta podrás conocer el sueldo</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Weldmation de México, S.A. de C.V.  en
+Ciudad de México</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Detalles
+Contratación:
+Tiempo completo
+Horario:
+Jornada completa
+Espacio de trabajo:
+						Presencial</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Descripción
+Requerimientos
+Educación mínima: Diplomado
+Objetivo del Rol
+Actuar como puente técnico entre el equipo interno de TI, el área de negocio y los equipos de desarrollo externos (DMS) facilitando la implementación eficiente de integraciones tecnológicas, garantizando seguridad, rendimiento y estabilidad en los sistemas.
+ Responsabilidades Técnicas?
+· 
+A
+nalizar, diseñar e implementar integraciones entre sistemas utilizando APIs (REST/JSON/XML) y protocolos de envío como SFTP.
+· Identificar y resolver proactivamente problemas técnicos relacionados con la configuración de integraciones e implementaciones.
+· Asegurar el cumplimiento de estándares de seguridad y rendimiento en las integraciones implementadas.
+· Participar activamente en las etapas del ciclo de vida del desarrollo de software, especialmente durante procesos de implementación y despliegue.
+· Colaborar con equipos técnicos de los distribuidores para definir soluciones de integración alineadas a los requerimientos del negocio.
+· Generar documentación técnica clara y precisa para facilitar la adopción y operación de las integraciones.
+· Brindar capacitación técnica a propietarios de aplicaciones del negocio y TI
+ en el 
+uso de herramientas y prácticas relacionadas con las integraciones.
+· Mantener comunicación directa con los equipos de TI de DTNA y DMS para resolución de incidencias y mejora continua.
+· Aplicar prácticas de trabajo bajo metodologías ágiles como Scrum para el seguimiento técnico de los desarrollos (deseable).
+Conocimientos y Herramientas Deseadas
+· API Management, Web Services, JSON, REST, XML.
+· Protocolos de comunicación seguros como SFTP.
+· Seguridad de integraciones (tokens, autenticación, certificados).
+· Control de versiones y herramientas de deployment (Git, CI/CD).
+· Experiencia en ambientes con múltiples sistemas y plataformas (DEV/QA/PRD).
+· Comprensión de metodologías ágiles (Scrum) y sus herramientas (Jira, Confluence, etc.).
+· Conocimiento amplio de herramientas de observabilidad y monitoreo (Splunk, ThosandEyes, Etc.)
+· Habilidad para entender procesos de negocio y transformarlos en un requerimiento técnico
+· Habilidades de comunicación efectiva
+· Experiencia en Industria Automotriz deseable.
+· Inglés mínimo B2</t>
         </is>
       </c>
     </row>

</xml_diff>